<commit_message>
updated dataproviders and etc..
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/nopData.xlsx
+++ b/src/test/resources/TestData/nopData.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Billing_Address" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="SearchProduct" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ProductQuantity" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="AccountCreationData" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t xml:space="preserve">email </t>
   </si>
@@ -75,14 +78,120 @@
   </si>
   <si>
     <t xml:space="preserve">Puram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenovo Thinkpad X1 Carbon Laptop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple MacBook Pro 13-inch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP Spectre XT Pro UltraBook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConfirmPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dinesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dineshkila99@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capgemini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dinesh123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nithya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nithyasri@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nithya123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raju</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajurajesh@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raju1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -176,7 +285,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,6 +308,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -284,7 +405,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.35"/>
   </cols>
@@ -366,11 +487,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -423,4 +544,263 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.35"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <f aca="false">SUM(1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
+        <f aca="false">SUM(3)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
+        <f aca="false">SUM(2)</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>1998</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1995</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>2001</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="dineshkila99@gmail.com"/>
+    <hyperlink ref="G3" r:id="rId2" display="nithyasri@gmail.com"/>
+    <hyperlink ref="G4" r:id="rId3" display="rajurajesh@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>